<commit_message>
combined expexperienced vol and master table into one
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/micro_reg_history_vol.xlsx
+++ b/WorkingFolder/Tables/micro_reg_history_vol.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>incvar I</t>
   </si>
@@ -34,127 +34,151 @@
     <t>inciqr III</t>
   </si>
   <si>
-    <t>rmse</t>
+    <t>exp_vol</t>
+  </si>
+  <si>
+    <t>age_gr=30-39</t>
+  </si>
+  <si>
+    <t>age_gr=40-48</t>
+  </si>
+  <si>
+    <t>age_gr=49-57</t>
+  </si>
+  <si>
+    <t>age_gr=&gt;57</t>
+  </si>
+  <si>
+    <t>educ_gr=low educ</t>
   </si>
   <si>
     <t>HHinc_gr=low inc</t>
   </si>
   <si>
-    <t>educ_gr=low educ</t>
-  </si>
-  <si>
-    <t>age_gr=30-39</t>
-  </si>
-  <si>
-    <t>age_gr=40-48</t>
-  </si>
-  <si>
-    <t>age_gr=49-57</t>
-  </si>
-  <si>
-    <t>age_gr=&gt;57</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>R2</t>
   </si>
   <si>
-    <t>4.02***</t>
-  </si>
-  <si>
-    <t>(0.25)</t>
+    <t>1.81***</t>
+  </si>
+  <si>
+    <t>(0.53)</t>
+  </si>
+  <si>
+    <t>-0.33***</t>
+  </si>
+  <si>
+    <t>(0.03)</t>
+  </si>
+  <si>
+    <t>-0.50***</t>
+  </si>
+  <si>
+    <t>-0.61***</t>
+  </si>
+  <si>
+    <t>-0.48***</t>
+  </si>
+  <si>
+    <t>(0.04)</t>
+  </si>
+  <si>
+    <t>40529</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>1.85***</t>
+  </si>
+  <si>
+    <t>-0.60***</t>
+  </si>
+  <si>
+    <t>-0.47***</t>
+  </si>
+  <si>
+    <t>-0.09***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>1.95***</t>
+  </si>
+  <si>
+    <t>-0.32***</t>
+  </si>
+  <si>
+    <t>-0.58***</t>
+  </si>
+  <si>
+    <t>-0.45***</t>
+  </si>
+  <si>
+    <t>-0.12***</t>
   </si>
   <si>
     <t>0.15***</t>
   </si>
   <si>
-    <t>(0.02)</t>
-  </si>
-  <si>
-    <t>40529</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
-    <t>3.82***</t>
-  </si>
-  <si>
-    <t>0.17***</t>
+    <t>0.96***</t>
+  </si>
+  <si>
+    <t>(0.29)</t>
+  </si>
+  <si>
+    <t>-0.17***</t>
+  </si>
+  <si>
+    <t>(0.01)</t>
+  </si>
+  <si>
+    <t>-0.25***</t>
+  </si>
+  <si>
+    <t>-0.30***</t>
+  </si>
+  <si>
+    <t>-0.23***</t>
+  </si>
+  <si>
+    <t>44874</t>
+  </si>
+  <si>
+    <t>0.94***</t>
+  </si>
+  <si>
+    <t>-0.26***</t>
+  </si>
+  <si>
+    <t>-0.31***</t>
+  </si>
+  <si>
+    <t>0.07***</t>
+  </si>
+  <si>
+    <t>1.05***</t>
+  </si>
+  <si>
+    <t>(0.28)</t>
   </si>
   <si>
     <t>-0.16***</t>
   </si>
   <si>
-    <t>1.95***</t>
-  </si>
-  <si>
-    <t>(0.53)</t>
-  </si>
-  <si>
-    <t>-0.12***</t>
-  </si>
-  <si>
-    <t>-0.32***</t>
-  </si>
-  <si>
-    <t>(0.03)</t>
-  </si>
-  <si>
-    <t>-0.48***</t>
-  </si>
-  <si>
-    <t>-0.58***</t>
-  </si>
-  <si>
-    <t>-0.45***</t>
-  </si>
-  <si>
-    <t>(0.04)</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>1.97***</t>
-  </si>
-  <si>
-    <t>(0.13)</t>
-  </si>
-  <si>
-    <t>0.20***</t>
-  </si>
-  <si>
-    <t>(0.01)</t>
-  </si>
-  <si>
-    <t>44874</t>
-  </si>
-  <si>
-    <t>1.99***</t>
-  </si>
-  <si>
-    <t>1.05***</t>
-  </si>
-  <si>
-    <t>(0.28)</t>
+    <t>-0.24***</t>
+  </si>
+  <si>
+    <t>-0.29***</t>
+  </si>
+  <si>
+    <t>0.03***</t>
   </si>
   <si>
     <t>0.19***</t>
-  </si>
-  <si>
-    <t>0.03***</t>
-  </si>
-  <si>
-    <t>-0.24***</t>
-  </si>
-  <si>
-    <t>-0.29***</t>
-  </si>
-  <si>
-    <t>-0.23***</t>
   </si>
   <si>
     <t>0.03</t>
@@ -549,19 +573,19 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -573,16 +597,16 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -593,19 +617,19 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -620,105 +644,177 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
       <c r="C7" t="s">
         <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1"/>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1"/>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -726,19 +822,19 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1"/>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -746,22 +842,22 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -769,22 +865,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved1. improved formatting. 2. added aggregate and idiosyncratic comparison.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/micro_reg_history_vol.xlsx
+++ b/WorkingFolder/Tables/micro_reg_history_vol.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="42">
   <si>
     <t>incvar I</t>
   </si>
@@ -67,106 +67,76 @@
     <t>(0.01)</t>
   </si>
   <si>
-    <t>-0.10***</t>
+    <t>-0.11***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>-0.16***</t>
   </si>
   <si>
     <t>-0.13***</t>
   </si>
   <si>
-    <t>-0.08***</t>
-  </si>
-  <si>
-    <t>0.41***</t>
-  </si>
-  <si>
-    <t>(0.16)</t>
-  </si>
-  <si>
-    <t>40529</t>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>41422</t>
   </si>
   <si>
     <t>0.01</t>
   </si>
   <si>
-    <t>-0.09***</t>
-  </si>
-  <si>
     <t>0.00</t>
   </si>
   <si>
     <t>(0.00)</t>
   </si>
   <si>
-    <t>-0.12***</t>
-  </si>
-  <si>
-    <t>-0.01**</t>
+    <t>-0.15***</t>
+  </si>
+  <si>
+    <t>-0.01</t>
   </si>
   <si>
     <t>0.06***</t>
   </si>
   <si>
-    <t>0.45***</t>
-  </si>
-  <si>
-    <t>-0.16***</t>
+    <t>-0.17***</t>
+  </si>
+  <si>
+    <t>-0.25***</t>
+  </si>
+  <si>
+    <t>(0.03)</t>
+  </si>
+  <si>
+    <t>-0.33***</t>
+  </si>
+  <si>
+    <t>-0.31***</t>
+  </si>
+  <si>
+    <t>44421</t>
+  </si>
+  <si>
+    <t>-0.26***</t>
+  </si>
+  <si>
+    <t>-0.34***</t>
+  </si>
+  <si>
+    <t>0.08***</t>
   </si>
   <si>
     <t>-0.24***</t>
   </si>
   <si>
-    <t>-0.28***</t>
-  </si>
-  <si>
-    <t>(0.02)</t>
-  </si>
-  <si>
-    <t>-0.22***</t>
-  </si>
-  <si>
-    <t>0.93***</t>
-  </si>
-  <si>
-    <t>(0.27)</t>
-  </si>
-  <si>
-    <t>44874</t>
-  </si>
-  <si>
-    <t>-0.25***</t>
-  </si>
-  <si>
-    <t>-0.30***</t>
-  </si>
-  <si>
-    <t>-0.23***</t>
-  </si>
-  <si>
-    <t>0.07***</t>
-  </si>
-  <si>
-    <t>0.90***</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>-0.15***</t>
-  </si>
-  <si>
-    <t>-0.27***</t>
-  </si>
-  <si>
-    <t>-0.21***</t>
-  </si>
-  <si>
-    <t>0.03***</t>
+    <t>0.04***</t>
   </si>
   <si>
     <t>0.18***</t>
-  </si>
-  <si>
-    <t>1.01***</t>
   </si>
   <si>
     <t>0.03</t>
@@ -567,13 +537,13 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -608,37 +578,37 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -646,43 +616,43 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -690,43 +660,43 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -734,25 +704,25 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1"/>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
@@ -766,16 +736,16 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
@@ -786,43 +756,43 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -839,13 +809,13 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -865,10 +835,10 @@
         <v>23</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>